<commit_message>
Some joint checks and minor modifications
</commit_message>
<xml_diff>
--- a/RSA_2019_08/X3_Data/x3_simpleRSA_KLandParams_20191221.xlsx
+++ b/RSA_2019_08/X3_Data/x3_simpleRSA_KLandParams_20191221.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="x3KLDivs_simpleRSA_indOpt_1STAR" sheetId="4" r:id="rId1"/>
@@ -1102,72 +1102,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1258,6 +1192,72 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1280,10 +1280,10 @@
   <tableColumns count="25">
     <tableColumn id="1" name="Spalte1"/>
     <tableColumn id="2" name="V1"/>
-    <tableColumn id="3" name="KL UB" dataDxfId="1"/>
+    <tableColumn id="3" name="KL UB" dataDxfId="8"/>
     <tableColumn id="4" name="KL gamma"/>
     <tableColumn id="5" name="KL beta"/>
-    <tableColumn id="6" name="KL lambda" dataDxfId="2"/>
+    <tableColumn id="6" name="KL lambda" dataDxfId="7"/>
     <tableColumn id="7" name="KL be la"/>
     <tableColumn id="8" name="KL ga la"/>
     <tableColumn id="9" name="KL ga be la"/>
@@ -1291,7 +1291,7 @@
     <tableColumn id="24" name="KL UB-Lamda">
       <calculatedColumnFormula>Tabelle15[[#This Row],[KL UB]]-Tabelle15[[#This Row],[KL lambda]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="AIC UB-AIC lambda" dataDxfId="0">
+    <tableColumn id="25" name="AIC UB-AIC lambda" dataDxfId="6">
       <calculatedColumnFormula>2*Tabelle15[[#This Row],[KL UB]]-2*Tabelle15[[#This Row],[KL lambda]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" name="KL L-GL">
@@ -1370,17 +1370,17 @@
     <tableColumn id="7" name="KL be la"/>
     <tableColumn id="8" name="KL ga la"/>
     <tableColumn id="9" name="KL ga be la"/>
-    <tableColumn id="10" name="KL_UB-GA_LA" dataDxfId="8">
+    <tableColumn id="10" name="KL_UB-GA_LA" dataDxfId="5">
       <calculatedColumnFormula>Tabelle14[[#This Row],[KL UB]]-Tabelle14[[#This Row],[KL ga la]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Spalte3" dataDxfId="7">
+    <tableColumn id="11" name="Spalte3" dataDxfId="4">
       <calculatedColumnFormula>Tabelle14[[#This Row],[KL lambda]]-Tabelle14[[#This Row],[KL ga la]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Spalte4" dataDxfId="6">
+    <tableColumn id="23" name="Spalte4" dataDxfId="3">
       <calculatedColumnFormula>MAX(Tabelle14[[#This Row],[Spalte3]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Spalte42" dataDxfId="5"/>
-    <tableColumn id="24" name="Spalte5" dataDxfId="4"/>
+    <tableColumn id="25" name="Spalte42" dataDxfId="2"/>
+    <tableColumn id="24" name="Spalte5" dataDxfId="1"/>
     <tableColumn id="12" name="V14"/>
     <tableColumn id="13" name="gamma"/>
     <tableColumn id="14" name="beta"/>
@@ -1413,7 +1413,7 @@
     <tableColumn id="7" name="KL be la"/>
     <tableColumn id="8" name="KL ga la"/>
     <tableColumn id="9" name="KL ga be la"/>
-    <tableColumn id="10" name="KL_UB-3Params" dataDxfId="3">
+    <tableColumn id="10" name="KL_UB-3Params" dataDxfId="0">
       <calculatedColumnFormula>Tabelle13[[#This Row],[KL UB]]-Tabelle13[[#This Row],[KL ga be la]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Spalte3"/>
@@ -1698,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y219"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L139" sqref="L139:L148"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14831,7 +14831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L137" sqref="L137"/>
     </sheetView>
   </sheetViews>

</xml_diff>